<commit_message>
Calculated start and finish line for all days #2
</commit_message>
<xml_diff>
--- a/data/filtered/Dati_filtrati_all.xlsx
+++ b/data/filtered/Dati_filtrati_all.xlsx
@@ -14,23 +14,32 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="97">
   <si>
     <t>Atleta</t>
   </si>
   <si>
-    <t>File</t>
+    <t>File from GPS</t>
+  </si>
+  <si>
+    <t>File Time</t>
   </si>
   <si>
     <t>Day</t>
   </si>
   <si>
+    <t>Time</t>
+  </si>
+  <si>
     <t>GPS matteo dnf</t>
   </si>
   <si>
     <t>../data/G1/0eb0781f-744c-450d-8d6b-e97a6b13d32a-resampled.csv</t>
   </si>
   <si>
+    <t>d9550d49-51cd-4f33-89b9-132229f94cc3</t>
+  </si>
+  <si>
     <t>G1</t>
   </si>
   <si>
@@ -40,18 +49,27 @@
     <t>../data/G1/213ae5cc-65f8-4930-a034-bf4dc2eae950-resampled.csv</t>
   </si>
   <si>
+    <t>8819f21a-e7cf-4902-8594-a99422a087cc</t>
+  </si>
+  <si>
     <t>GPS martin</t>
   </si>
   <si>
     <t>../data/G1/2669730a-67a2-48c7-818b-5cd2ecfec89d-resampled.csv</t>
   </si>
   <si>
+    <t>6f86baa4-baef-45b9-91a9-03d5297ff828</t>
+  </si>
+  <si>
     <t>GPS meggye</t>
   </si>
   <si>
     <t>../data/G1/303af368-a921-454b-a05c-76799c9c8021-resampled.csv</t>
   </si>
   <si>
+    <t>0d3cdd18-8bb6-421c-9727-6493132512f8</t>
+  </si>
+  <si>
     <t>../data/G1/6a81168d-4940-48c5-8981-bd809fb6ebf5-resampled.csv</t>
   </si>
   <si>
@@ -61,42 +79,66 @@
     <t>../data/G1/7146465b-ba5c-4300-af0c-043e579c13bc-resampled.csv</t>
   </si>
   <si>
+    <t>e55c6c13-8ad4-4f27-8509-2627c7e15000</t>
+  </si>
+  <si>
     <t>../data/G1/7af9a467-b0b8-4636-81ae-f47fca403b0c-resampled.csv</t>
   </si>
   <si>
+    <t>aaa56591-e0e4-47df-9f65-391cba7dc264</t>
+  </si>
+  <si>
     <t>GPS Ilaria</t>
   </si>
   <si>
     <t>../data/G1/85e148df-0b3c-4994-82d2-ac033a3167e5-resampled.csv</t>
   </si>
   <si>
+    <t>9b1cf9ec-e798-4a4a-896f-289963344901</t>
+  </si>
+  <si>
     <t>GPS aydan</t>
   </si>
   <si>
     <t>../data/G1/92cfda15-66c1-4f84-8123-e0ed1135d1e2-resampled.csv</t>
   </si>
   <si>
+    <t>711af94b-32fc-4a3e-a57c-94094576a647</t>
+  </si>
+  <si>
     <t>GPS ela2</t>
   </si>
   <si>
     <t>../data/G1/9348535c-147a-4553-9860-e10e2b168502-resampled.csv</t>
   </si>
   <si>
+    <t>7d9194df-cc41-4776-bdbf-9b53a667eb5e</t>
+  </si>
+  <si>
     <t>GPS giorgio</t>
   </si>
   <si>
     <t>../data/G1/9f86ac8b-d9b5-4623-aada-b4557ec160fe-resampled.csv</t>
   </si>
   <si>
+    <t>ecdddfb7-360d-47c3-b287-6f004790ec0f</t>
+  </si>
+  <si>
     <t>../data/G1/a8b20cfa-e7dd-41f6-a184-31351cb9d875-resampled.csv</t>
   </si>
   <si>
+    <t>219be45d-395b-4166-83a4-dd9424d07a29</t>
+  </si>
+  <si>
     <t>GPS bea</t>
   </si>
   <si>
     <t>../data/G1/be5e753b-2fd1-45c1-b101-3a969c8611a6-resampled.csv</t>
   </si>
   <si>
+    <t>20062c55-4adb-4fc8-8674-7bbd9b582e51</t>
+  </si>
+  <si>
     <t>../data/G1/c50fd215-01c8-4948-9c4e-9133696d494f-resampled.csv</t>
   </si>
   <si>
@@ -115,6 +157,9 @@
     <t>../data/P1/1a50d4b0-e1db-498d-99f1-9b09b2ea2c66-resampled.csv</t>
   </si>
   <si>
+    <t>af90cde0-bba7-4800-bbdf-b77c9a1e857e</t>
+  </si>
+  <si>
     <t>P1</t>
   </si>
   <si>
@@ -124,91 +169,142 @@
     <t>../data/P1/7b9b3882-d9c8-4d74-b6f3-92d15fd5d031-resampled.csv</t>
   </si>
   <si>
+    <t>7d631690-0ff8-4ee2-b924-aec61844a67a</t>
+  </si>
+  <si>
     <t>GPS Cate</t>
   </si>
   <si>
     <t>../data/P1/7c85e503-8287-4e2c-b69f-ac9e8a9b2cb8-resampled.csv</t>
   </si>
   <si>
+    <t>933a5140-9397-4506-9c69-d2f6d25901cd</t>
+  </si>
+  <si>
     <t>GPS Gal</t>
   </si>
   <si>
     <t>../data/P1/8f53a4f1-b0fe-47d0-8dbb-1ecc29b8d384-resampled.csv</t>
   </si>
   <si>
+    <t>891df5aa-0df9-4676-b4c2-492db382a1fd</t>
+  </si>
+  <si>
     <t>GPS Bea</t>
   </si>
   <si>
     <t>../data/P1/a428c925-034d-4119-974d-3626dad5eafe-resampled.csv</t>
   </si>
   <si>
+    <t>d4dbc3ba-2ad6-489a-bacb-61c7fbd5317d</t>
+  </si>
+  <si>
     <t>GPS Jelenček</t>
   </si>
   <si>
     <t>../data/P1/ae2ecfac-610f-473d-81b4-927d3654bca9-resampled.csv</t>
   </si>
   <si>
+    <t>01478c9d-61b6-4252-be0e-211d1fd830bf</t>
+  </si>
+  <si>
     <t>../data/P1/d3b79fa1-459e-4b36-b4d9-c28ab53de2f9-resampled.csv</t>
   </si>
   <si>
+    <t>eeadc2dc-8075-4b09-8821-ebb9edad7ddf</t>
+  </si>
+  <si>
     <t>../data/P1/d8e68817-55d8-4407-a726-dc5149d2ab6b-resampled.csv</t>
   </si>
   <si>
+    <t>eef9af7b-68d6-423e-907b-d43ef258440e</t>
+  </si>
+  <si>
     <t>GPS Nik</t>
   </si>
   <si>
     <t>../data/P1/e8aa40a3-9f54-4d8b-bc6c-ab0369ce9903-resampled.csv</t>
   </si>
   <si>
+    <t>51dac331-4ab1-4f29-b828-a278af3298d8</t>
+  </si>
+  <si>
     <t>GPS Manca</t>
   </si>
   <si>
     <t>../data/P2/02d7d896-e139-4bec-b8e1-325d995784ac-resampled.csv</t>
   </si>
   <si>
+    <t>0657cdd4-77d4-4531-9f39-b814c18fef57</t>
+  </si>
+  <si>
     <t>P2</t>
   </si>
   <si>
     <t>../data/P2/08c2eb3d-6378-4723-b279-ba1dd9707539-resampled.csv</t>
   </si>
   <si>
+    <t>c267dd15-7963-45eb-8f50-cecad9bdac5e</t>
+  </si>
+  <si>
     <t>GPS gal</t>
   </si>
   <si>
     <t>../data/P2/0c65d602-1d78-4928-8479-ecf7f379c96b-resampled.csv</t>
   </si>
   <si>
+    <t>bcb01797-4372-4e5c-8fab-133013e674a2</t>
+  </si>
+  <si>
     <t>GPS chiara</t>
   </si>
   <si>
     <t>../data/P2/445506b6-d3c2-4652-8bb0-d4710bc29060-resampled.csv</t>
   </si>
   <si>
+    <t>a9e51f8f-eec9-4fa9-a67e-389333b82516</t>
+  </si>
+  <si>
     <t>../data/P2/826e4d89-1893-4340-9a5b-e1aaee3d9d5d-resampled.csv</t>
   </si>
   <si>
+    <t>987622c6-63a0-4f82-8694-9ddf894141c8</t>
+  </si>
+  <si>
     <t>GPS Francesco</t>
   </si>
   <si>
     <t>../data/P2/aec20d08-f114-4f63-87e1-23a6181456ef-resampled.csv</t>
   </si>
   <si>
+    <t>076c15b5-6249-44fa-8a5f-17f87f7473de</t>
+  </si>
+  <si>
     <t>GPS Zavattarelli DNF</t>
   </si>
   <si>
     <t>../data/P2/b2a77a61-db79-47c7-8ccd-40c86b37eeeb-resampled.csv</t>
   </si>
   <si>
+    <t>60e4a812-4955-49ca-9cf1-db7286bcd6e6</t>
+  </si>
+  <si>
     <t>../data/P2/bf87b2f3-9e81-438a-90cf-7046750c2ebd-resampled.csv</t>
   </si>
   <si>
     <t>../data/P2/dacec0b0-7f24-4e92-bba3-e5b6e8649b90-resampled.csv</t>
   </si>
   <si>
+    <t>10a190b4-06ef-4803-8d5f-23dacf9ceec1</t>
+  </si>
+  <si>
     <t>GPS Sofia</t>
   </si>
   <si>
     <t>../data/P2/fed06dd6-c72c-477f-8778-23ca991ce4ea-resampled.csv</t>
+  </si>
+  <si>
+    <t>41546c9b-b81e-45a9-9cd8-58aebd621714</t>
   </si>
 </sst>
 </file>
@@ -540,13 +636,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -556,401 +652,623 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2">
+        <v>43.93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3">
+        <v>45.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4">
+        <v>44.04</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5">
+        <v>48.65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6">
+        <v>48.65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7">
+        <v>44.45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
         <v>12</v>
       </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>23</v>
+      </c>
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8">
+        <v>43.38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>26</v>
+      </c>
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9">
+        <v>47.19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+        <v>29</v>
+      </c>
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10">
+        <v>45.54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="C11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>32</v>
+      </c>
+      <c r="D11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11">
+        <v>45.37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12">
+        <v>46.01</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13">
+        <v>47.46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14">
+        <v>44.89</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" t="s">
         <v>23</v>
       </c>
-      <c r="C12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="D15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15">
+        <v>43.38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
         <v>24</v>
       </c>
-      <c r="C13" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="B16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" t="s">
         <v>26</v>
       </c>
-      <c r="C14" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="D16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16">
+        <v>47.19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="C17" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
+        <v>32</v>
+      </c>
+      <c r="D17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17">
+        <v>45.37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="B18" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="C18" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
+        <v>40</v>
+      </c>
+      <c r="D18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18">
+        <v>44.89</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="B19" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="C19" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
+        <v>47</v>
+      </c>
+      <c r="D19" t="s">
+        <v>48</v>
+      </c>
+      <c r="E19">
+        <v>35.62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="B20" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C20" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
+        <v>51</v>
+      </c>
+      <c r="D20" t="s">
+        <v>48</v>
+      </c>
+      <c r="E20">
+        <v>37.96</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="B21" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="C21" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
+        <v>54</v>
+      </c>
+      <c r="D21" t="s">
+        <v>48</v>
+      </c>
+      <c r="E21">
+        <v>35.91</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" t="s">
+        <v>57</v>
+      </c>
+      <c r="D22" t="s">
+        <v>48</v>
+      </c>
+      <c r="E22">
+        <v>35.2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" t="s">
+        <v>60</v>
+      </c>
+      <c r="D23" t="s">
+        <v>48</v>
+      </c>
+      <c r="E23">
+        <v>35.95</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24" t="s">
+        <v>62</v>
+      </c>
+      <c r="C24" t="s">
+        <v>63</v>
+      </c>
+      <c r="D24" t="s">
+        <v>48</v>
+      </c>
+      <c r="E24">
+        <v>39.38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" t="s">
+        <v>52</v>
+      </c>
+      <c r="B25" t="s">
+        <v>64</v>
+      </c>
+      <c r="C25" t="s">
+        <v>65</v>
+      </c>
+      <c r="D25" t="s">
+        <v>48</v>
+      </c>
+      <c r="E25">
+        <v>35.3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" t="s">
+        <v>66</v>
+      </c>
+      <c r="C26" t="s">
+        <v>67</v>
+      </c>
+      <c r="D26" t="s">
+        <v>48</v>
+      </c>
+      <c r="E26">
+        <v>36.72</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" t="s">
+        <v>68</v>
+      </c>
+      <c r="B27" t="s">
+        <v>69</v>
+      </c>
+      <c r="C27" t="s">
+        <v>70</v>
+      </c>
+      <c r="D27" t="s">
+        <v>48</v>
+      </c>
+      <c r="E27">
+        <v>37.84</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" t="s">
+        <v>71</v>
+      </c>
+      <c r="B28" t="s">
+        <v>72</v>
+      </c>
+      <c r="C28" t="s">
+        <v>73</v>
+      </c>
+      <c r="D28" t="s">
+        <v>74</v>
+      </c>
+      <c r="E28">
+        <v>39.01</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" t="s">
+        <v>45</v>
+      </c>
+      <c r="B29" t="s">
+        <v>75</v>
+      </c>
+      <c r="C29" t="s">
+        <v>76</v>
+      </c>
+      <c r="D29" t="s">
+        <v>74</v>
+      </c>
+      <c r="E29">
+        <v>35.77</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" t="s">
+        <v>77</v>
+      </c>
+      <c r="B30" t="s">
+        <v>78</v>
+      </c>
+      <c r="C30" t="s">
+        <v>79</v>
+      </c>
+      <c r="D30" t="s">
+        <v>74</v>
+      </c>
+      <c r="E30">
+        <v>35.47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" t="s">
+        <v>80</v>
+      </c>
+      <c r="B31" t="s">
+        <v>81</v>
+      </c>
+      <c r="C31" t="s">
+        <v>82</v>
+      </c>
+      <c r="D31" t="s">
+        <v>74</v>
+      </c>
+      <c r="E31">
+        <v>35.73</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" t="s">
+        <v>52</v>
+      </c>
+      <c r="B32" t="s">
+        <v>83</v>
+      </c>
+      <c r="C32" t="s">
+        <v>84</v>
+      </c>
+      <c r="D32" t="s">
+        <v>74</v>
+      </c>
+      <c r="E32">
+        <v>35.03</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" t="s">
+        <v>85</v>
+      </c>
+      <c r="B33" t="s">
+        <v>86</v>
+      </c>
+      <c r="C33" t="s">
+        <v>87</v>
+      </c>
+      <c r="D33" t="s">
+        <v>74</v>
+      </c>
+      <c r="E33">
+        <v>35.01</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" t="s">
+        <v>88</v>
+      </c>
+      <c r="B34" t="s">
+        <v>89</v>
+      </c>
+      <c r="C34" t="s">
+        <v>90</v>
+      </c>
+      <c r="D34" t="s">
+        <v>74</v>
+      </c>
+      <c r="E34">
+        <v>35.98</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" t="s">
+        <v>80</v>
+      </c>
+      <c r="B35" t="s">
+        <v>91</v>
+      </c>
+      <c r="C35" t="s">
+        <v>82</v>
+      </c>
+      <c r="D35" t="s">
+        <v>74</v>
+      </c>
+      <c r="E35">
+        <v>35.73</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" t="s">
         <v>38</v>
       </c>
-      <c r="B22" t="s">
-        <v>39</v>
-      </c>
-      <c r="C22" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" t="s">
-        <v>40</v>
-      </c>
-      <c r="B23" t="s">
-        <v>41</v>
-      </c>
-      <c r="C23" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" t="s">
-        <v>42</v>
-      </c>
-      <c r="B24" t="s">
-        <v>43</v>
-      </c>
-      <c r="C24" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" t="s">
-        <v>36</v>
-      </c>
-      <c r="B25" t="s">
-        <v>44</v>
-      </c>
-      <c r="C25" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" t="s">
-        <v>40</v>
-      </c>
-      <c r="B26" t="s">
-        <v>45</v>
-      </c>
-      <c r="C26" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" t="s">
-        <v>46</v>
-      </c>
-      <c r="B27" t="s">
-        <v>47</v>
-      </c>
-      <c r="C27" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" t="s">
-        <v>48</v>
-      </c>
-      <c r="B28" t="s">
-        <v>49</v>
-      </c>
-      <c r="C28" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" t="s">
-        <v>31</v>
-      </c>
-      <c r="B29" t="s">
-        <v>51</v>
-      </c>
-      <c r="C29" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" t="s">
-        <v>52</v>
-      </c>
-      <c r="B30" t="s">
-        <v>53</v>
-      </c>
-      <c r="C30" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" t="s">
-        <v>54</v>
-      </c>
-      <c r="B31" t="s">
-        <v>55</v>
-      </c>
-      <c r="C31" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" t="s">
-        <v>36</v>
-      </c>
-      <c r="B32" t="s">
-        <v>56</v>
-      </c>
-      <c r="C32" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" t="s">
-        <v>57</v>
-      </c>
-      <c r="B33" t="s">
-        <v>58</v>
-      </c>
-      <c r="C33" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" t="s">
-        <v>59</v>
-      </c>
-      <c r="B34" t="s">
-        <v>60</v>
-      </c>
-      <c r="C34" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" t="s">
-        <v>54</v>
-      </c>
-      <c r="B35" t="s">
-        <v>61</v>
-      </c>
-      <c r="C35" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" t="s">
-        <v>25</v>
-      </c>
       <c r="B36" t="s">
-        <v>62</v>
+        <v>92</v>
       </c>
       <c r="C36" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
+        <v>93</v>
+      </c>
+      <c r="D36" t="s">
+        <v>74</v>
+      </c>
+      <c r="E36">
+        <v>36.25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
       <c r="A37" t="s">
-        <v>63</v>
+        <v>94</v>
       </c>
       <c r="B37" t="s">
-        <v>64</v>
+        <v>95</v>
       </c>
       <c r="C37" t="s">
-        <v>50</v>
+        <v>96</v>
+      </c>
+      <c r="D37" t="s">
+        <v>74</v>
+      </c>
+      <c r="E37">
+        <v>37.61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>